<commit_message>
done with Program 8
</commit_message>
<xml_diff>
--- a/Program8/Results.xlsx
+++ b/Program8/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\NMSU\CS471\Program8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491309F6-A55E-442D-B442-6098AD729706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC49892E-502C-4A31-8917-CCC92FFBA287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -192,7 +192,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -204,7 +203,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -383,16 +381,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0654999999999999</c:v>
+                  <c:v>0.78450399999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5320800000000001</c:v>
+                  <c:v>0.81005440000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3354200000000001</c:v>
+                  <c:v>1.1508201999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0590799999999998</c:v>
+                  <c:v>1.5981031999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1533,10 +1531,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1554,7 @@
       <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D1" t="s">
@@ -1564,369 +1565,369 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6">
         <v>2</v>
       </c>
-      <c r="C2" s="10">
-        <v>1159900</v>
+      <c r="C2" s="9">
+        <v>1795928</v>
       </c>
       <c r="D2" s="6">
         <f>C2/1000</f>
-        <v>1159.9000000000001</v>
+        <v>1795.9280000000001</v>
       </c>
       <c r="E2" s="6">
         <f>C2/1000000</f>
-        <v>1.1598999999999999</v>
+        <v>1.795928</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="6">
         <v>4</v>
       </c>
-      <c r="C3" s="10">
-        <v>1658500</v>
+      <c r="C3" s="9">
+        <v>974073</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D35" si="0">C3/1000</f>
-        <v>1658.5</v>
+        <v>974.07299999999998</v>
       </c>
       <c r="E3" s="6">
         <f t="shared" ref="E3:E34" si="1">C3/1000000</f>
-        <v>1.6585000000000001</v>
+        <v>0.97407299999999997</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="6">
         <v>8</v>
       </c>
-      <c r="C4" s="11">
-        <v>2270200</v>
+      <c r="C4" s="10">
+        <v>1035084</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>2270.1999999999998</v>
+        <v>1035.0840000000001</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" si="1"/>
-        <v>2.2702</v>
+        <v>1.0350839999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="6">
         <v>16</v>
       </c>
-      <c r="C5" s="11">
-        <v>4462400</v>
+      <c r="C5" s="10">
+        <v>1626093</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>4462.3999999999996</v>
+        <v>1626.0930000000001</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="1"/>
-        <v>4.4623999999999997</v>
+        <v>1.626093</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="C7" s="11">
-        <v>1081500</v>
+      <c r="C7" s="10">
+        <v>652631</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>1081.5</v>
+        <v>652.63099999999997</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="1"/>
-        <v>1.0814999999999999</v>
+        <v>0.65263099999999996</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="11">
-        <v>1647300</v>
+      <c r="C8" s="10">
+        <v>767637</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>1647.3</v>
+        <v>767.63699999999994</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" si="1"/>
-        <v>1.6473</v>
+        <v>0.76763700000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="6">
         <v>8</v>
       </c>
-      <c r="C9" s="10">
-        <v>2579800</v>
+      <c r="C9" s="9">
+        <v>1193956</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>2579.8000000000002</v>
+        <v>1193.9559999999999</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="1"/>
-        <v>2.5798000000000001</v>
+        <v>1.193956</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="6">
         <v>16</v>
       </c>
-      <c r="C10" s="10">
-        <v>4623000</v>
+      <c r="C10" s="9">
+        <v>1645465</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
-        <v>4623</v>
+        <v>1645.4649999999999</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="1"/>
-        <v>4.6230000000000002</v>
+        <v>1.645465</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="10">
-        <v>1167500</v>
+      <c r="C12" s="9">
+        <v>378355</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="0"/>
-        <v>1167.5</v>
+        <v>378.35500000000002</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="1"/>
-        <v>1.1675</v>
+        <v>0.378355</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="6">
         <v>4</v>
       </c>
-      <c r="C13" s="10">
-        <v>1537600</v>
+      <c r="C13" s="9">
+        <v>725574</v>
       </c>
       <c r="D13" s="6">
         <f t="shared" si="0"/>
-        <v>1537.6</v>
+        <v>725.57399999999996</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" si="1"/>
-        <v>1.5376000000000001</v>
+        <v>0.72557400000000005</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="6">
         <v>8</v>
       </c>
-      <c r="C14" s="10">
-        <v>2330600</v>
+      <c r="C14" s="9">
+        <v>1005584</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="0"/>
-        <v>2330.6</v>
+        <v>1005.5839999999999</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" si="1"/>
-        <v>2.3306</v>
+        <v>1.005584</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="6">
         <v>16</v>
       </c>
-      <c r="C15" s="10">
-        <v>4050200</v>
+      <c r="C15" s="9">
+        <v>1666428</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="0"/>
-        <v>4050.2</v>
+        <v>1666.4280000000001</v>
       </c>
       <c r="E15" s="6">
         <f t="shared" si="1"/>
-        <v>4.0502000000000002</v>
+        <v>1.666428</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="10">
-        <v>957900</v>
+      <c r="C17" s="9">
+        <v>557455</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="0"/>
-        <v>957.9</v>
+        <v>557.45500000000004</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="1"/>
-        <v>0.95789999999999997</v>
+        <v>0.55745500000000003</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="6">
         <v>4</v>
       </c>
-      <c r="C18" s="10">
-        <v>1383600</v>
+      <c r="C18" s="9">
+        <v>804092</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="0"/>
-        <v>1383.6</v>
+        <v>804.09199999999998</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="1"/>
-        <v>1.3835999999999999</v>
+        <v>0.80409200000000003</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="6">
         <v>8</v>
       </c>
-      <c r="C19" s="10">
-        <v>2364100</v>
+      <c r="C19" s="9">
+        <v>1286410</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="0"/>
-        <v>2364.1</v>
+        <v>1286.4100000000001</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" si="1"/>
-        <v>2.3641000000000001</v>
+        <v>1.2864100000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="6">
         <v>16</v>
       </c>
-      <c r="C20" s="10">
-        <v>3534200</v>
+      <c r="C20" s="9">
+        <v>1665436</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" si="0"/>
-        <v>3534.2</v>
+        <v>1665.4359999999999</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="1"/>
-        <v>3.5341999999999998</v>
+        <v>1.6654359999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="10">
-        <v>960700</v>
+      <c r="C22" s="9">
+        <v>538151</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="0"/>
-        <v>960.7</v>
+        <v>538.15099999999995</v>
       </c>
       <c r="E22" s="6">
         <f t="shared" si="1"/>
-        <v>0.9607</v>
+        <v>0.53815100000000005</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="6">
         <v>4</v>
       </c>
-      <c r="C23" s="10">
-        <v>1433400</v>
+      <c r="C23" s="9">
+        <v>778896</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="0"/>
-        <v>1433.4</v>
+        <v>778.89599999999996</v>
       </c>
       <c r="E23" s="6">
         <f t="shared" si="1"/>
-        <v>1.4334</v>
+        <v>0.77889600000000003</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="6">
         <v>8</v>
       </c>
-      <c r="C24" s="10">
-        <v>2132400</v>
+      <c r="C24" s="9">
+        <v>1233067</v>
       </c>
       <c r="D24" s="6">
         <f t="shared" si="0"/>
-        <v>2132.4</v>
+        <v>1233.067</v>
       </c>
       <c r="E24" s="6">
         <f t="shared" si="1"/>
-        <v>2.1324000000000001</v>
+        <v>1.2330669999999999</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="6">
         <v>16</v>
       </c>
-      <c r="C25" s="10">
-        <v>3625600</v>
+      <c r="C25" s="9">
+        <v>1387094</v>
       </c>
       <c r="D25" s="6">
         <f t="shared" si="0"/>
-        <v>3625.6</v>
+        <v>1387.0940000000001</v>
       </c>
       <c r="E25" s="6">
         <f t="shared" si="1"/>
-        <v>3.6255999999999999</v>
+        <v>1.387094</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="4">
@@ -1934,153 +1935,153 @@
       </c>
       <c r="C27" s="5">
         <f>AVERAGE(C2,C7,C12,C17,C22)</f>
-        <v>1065500</v>
+        <v>784504</v>
       </c>
       <c r="D27" s="4">
         <f>C27/1000</f>
-        <v>1065.5</v>
+        <v>784.50400000000002</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="1"/>
-        <v>1.0654999999999999</v>
+        <v>0.78450399999999998</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="4">
         <v>4</v>
       </c>
       <c r="C28" s="5">
         <f>AVERAGE(C3,C8,C13,C18,C23)</f>
-        <v>1532080</v>
+        <v>810054.4</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="0"/>
-        <v>1532.08</v>
+        <v>810.05439999999999</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="1"/>
-        <v>1.5320800000000001</v>
+        <v>0.81005440000000006</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="4">
         <v>8</v>
       </c>
       <c r="C29" s="5">
         <f>AVERAGE(C4,C9,C14,C19,C24)</f>
-        <v>2335420</v>
+        <v>1150820.2</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="0"/>
-        <v>2335.42</v>
+        <v>1150.8201999999999</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="1"/>
-        <v>2.3354200000000001</v>
+        <v>1.1508201999999998</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="4">
         <v>16</v>
       </c>
       <c r="C30" s="5">
         <f>AVERAGE(C5,C10,C15,C20,C25)</f>
-        <v>4059080</v>
+        <v>1598103.2</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="0"/>
-        <v>4059.08</v>
+        <v>1598.1032</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="1"/>
-        <v>4.0590799999999998</v>
+        <v>1.5981031999999999</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="19"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="17"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="7">
         <v>2</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <f>STDEV(C2,C7,C12,C17,C22)</f>
-        <v>102630.59972542302</v>
-      </c>
-      <c r="D32" s="8">
-        <f t="shared" si="0"/>
-        <v>102.63059972542301</v>
-      </c>
-      <c r="E32" s="8">
-        <f t="shared" si="1"/>
-        <v>0.10263059972542302</v>
+        <v>573926.61881027964</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>573.92661881027959</v>
+      </c>
+      <c r="E32" s="7">
+        <f t="shared" si="1"/>
+        <v>0.57392661881027962</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="8">
+      <c r="A33" s="16"/>
+      <c r="B33" s="7">
         <v>4</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <f>STDEV(C3,C8,C13,C18,C23)</f>
-        <v>123563.93891423177</v>
-      </c>
-      <c r="D33" s="8">
-        <f t="shared" si="0"/>
-        <v>123.56393891423177</v>
-      </c>
-      <c r="E33" s="8">
-        <f t="shared" si="1"/>
-        <v>0.12356393891423177</v>
+        <v>95974.828805786616</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="0"/>
+        <v>95.974828805786615</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" si="1"/>
+        <v>9.5974828805786616E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="8">
+      <c r="A34" s="16"/>
+      <c r="B34" s="7">
         <v>8</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <f>STDEV(C4,C9,C14,C19,C24)</f>
-        <v>162817.4806339909</v>
-      </c>
-      <c r="D34" s="8">
-        <f t="shared" si="0"/>
-        <v>162.8174806339909</v>
-      </c>
-      <c r="E34" s="8">
-        <f t="shared" si="1"/>
-        <v>0.1628174806339909</v>
+        <v>123994.20248221286</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="0"/>
+        <v>123.99420248221286</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" si="1"/>
+        <v>0.12399420248221286</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="8">
+      <c r="A35" s="19"/>
+      <c r="B35" s="7">
         <v>16</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <f>STDEV(C5,C10,C15,C20,C25)</f>
-        <v>485838.33936814824</v>
-      </c>
-      <c r="D35" s="8">
-        <f t="shared" si="0"/>
-        <v>485.83833936814824</v>
-      </c>
-      <c r="E35" s="8">
+        <v>119114.89803840659</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="0"/>
+        <v>119.11489803840659</v>
+      </c>
+      <c r="E35" s="7">
         <f>C35/1000000</f>
-        <v>0.48583833936814824</v>
+        <v>0.11911489803840659</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="56" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>